<commit_message>
oracle init database first version done
</commit_message>
<xml_diff>
--- a/test/schema/systems.xlsx
+++ b/test/schema/systems.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="4040" windowWidth="25340" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,10 +34,6 @@
   </si>
   <si>
     <t>Password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin00!!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -123,21 +119,18 @@
     <t>游戏系统配置</t>
   </si>
   <si>
+    <t>test_game_system</t>
+  </si>
+  <si>
+    <t>test_game_logDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>localhost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>gameAdmin2</t>
-  </si>
-  <si>
-    <t>test_game_system</t>
-  </si>
-  <si>
-    <t>test_game_logDB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>localhost</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gameAdmin2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -155,6 +148,21 @@
   <si>
     <t>游戏服务器大区配置</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gameAdmin1</t>
+  </si>
+  <si>
+    <t>gameAdmin3</t>
+  </si>
+  <si>
+    <t>admin01</t>
+  </si>
+  <si>
+    <t>admin02</t>
+  </si>
+  <si>
+    <t>admin03</t>
   </si>
 </sst>
 </file>
@@ -165,14 +173,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -180,14 +188,14 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -196,7 +204,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -205,7 +213,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -218,7 +226,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -349,21 +357,21 @@
     </xf>
   </cellXfs>
   <cellStyles count="15">
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -712,14 +720,14 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -731,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
@@ -740,76 +748,75 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.5" customHeight="1">
       <c r="A3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13.5" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="F4" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -838,30 +845,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12">
       <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="4" t="b">
         <v>1</v>
@@ -870,13 +877,13 @@
     </row>
     <row r="3" spans="1:5" ht="12">
       <c r="A3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="b">
         <v>1</v>
@@ -885,10 +892,10 @@
     </row>
     <row r="4" spans="1:5" ht="12">
       <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -896,13 +903,13 @@
     </row>
     <row r="5" spans="1:5" ht="13.5" customHeight="1">
       <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>

</xml_diff>